<commit_message>
add glaucoma progression paper exclusions, add medications and SLT
</commit_message>
<xml_diff>
--- a/codes/progression_surgery_codes_outcomes.xlsx
+++ b/codes/progression_surgery_codes_outcomes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoa-my.sharepoint.com/personal/ahol834_uoa_auckland_ac_nz/Documents/Hons/Progression ML paper/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/resmed202100066-Glaucoma_PRS/andrewholmes2024/summer2025/outcomes/codes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="247" documentId="8_{33FF13D1-89AE-0345-AAFF-D866902A6AB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{817036FA-8FF7-2E4F-BCD5-BABE5FC29386}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C4F39F-D868-2C45-85E8-763CA7548A37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="18360" activeTab="1" xr2:uid="{50CFBF05-B7E9-BF4A-8961-70BF8FF71AD6}"/>
+    <workbookView xWindow="-4660" yWindow="-21100" windowWidth="25600" windowHeight="21100" xr2:uid="{50CFBF05-B7E9-BF4A-8961-70BF8FF71AD6}"/>
   </bookViews>
   <sheets>
     <sheet name="opcs4_inpatient" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="94">
   <si>
     <t>Corneoscleral trephine</t>
   </si>
@@ -80,18 +80,6 @@
     <t>Other operations on trabecular meshwork of eye</t>
   </si>
   <si>
-    <t>72561</t>
-  </si>
-  <si>
-    <t>Trabeculotomy</t>
-  </si>
-  <si>
-    <t>72562</t>
-  </si>
-  <si>
-    <t>Goniotomy</t>
-  </si>
-  <si>
     <t>7256y</t>
   </si>
   <si>
@@ -176,9 +164,6 @@
     <t>Insertion of drainage tube into anterior chamber</t>
   </si>
   <si>
-    <t>XE0BO</t>
-  </si>
-  <si>
     <t>XaJdX</t>
   </si>
   <si>
@@ -236,18 +221,6 @@
     <t>C60.6 Viscocanulostomy</t>
   </si>
   <si>
-    <t>C612</t>
-  </si>
-  <si>
-    <t>C61.2 Trabeculotomy</t>
-  </si>
-  <si>
-    <t>C613</t>
-  </si>
-  <si>
-    <t>C61.3 Goniotomy</t>
-  </si>
-  <si>
     <t>C618</t>
   </si>
   <si>
@@ -272,9 +245,6 @@
     <t>C52.2 Deep sclerectomy without spacer</t>
   </si>
   <si>
-    <t>157.3 Destruction of ciliary body : goniotomy</t>
-  </si>
-  <si>
     <t>157.4 Destruction of ciliary body : trabeculectomy</t>
   </si>
   <si>
@@ -311,21 +281,12 @@
     <t>I</t>
   </si>
   <si>
-    <t>MIGS </t>
-  </si>
-  <si>
-    <t>D, MIGS</t>
-  </si>
-  <si>
     <t>I, MIGS, D</t>
   </si>
   <si>
     <t>162 Corneo-scleral trephine and  sclerotomy</t>
   </si>
   <si>
-    <t>MIGS</t>
-  </si>
-  <si>
     <t>D</t>
   </si>
   <si>
@@ -342,6 +303,24 @@
   </si>
   <si>
     <t>Creation of guarded fistula to sclera (OPCS4 C601) </t>
+  </si>
+  <si>
+    <t>D, MIGS </t>
+  </si>
+  <si>
+    <t>I, MIGS, D </t>
+  </si>
+  <si>
+    <t>XE0BJ</t>
+  </si>
+  <si>
+    <t>Trephining of sclera and iridectomy</t>
+  </si>
+  <si>
+    <t>Xa9R5</t>
+  </si>
+  <si>
+    <t>Anterior chamber drainage tube</t>
   </si>
 </sst>
 </file>
@@ -351,17 +330,10 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -393,12 +365,11 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -416,10 +387,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -739,10 +706,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60CF15B7-22DE-5845-80EA-57A73503675F}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView zoomScale="156" workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:C1"/>
+    <sheetView tabSelected="1" zoomScale="156" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -753,112 +720,90 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B1" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="C1" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C2" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="C3" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C4" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B6" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C6" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B8" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>69</v>
-      </c>
-      <c r="B9" t="s">
-        <v>70</v>
-      </c>
-      <c r="C9" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>71</v>
-      </c>
-      <c r="B10" t="s">
-        <v>72</v>
-      </c>
-      <c r="C10" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -868,70 +813,59 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDF8FE3F-34F6-7641-850C-2F75927AEE33}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView zoomScale="110" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="50.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B1" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="C1" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
+      <c r="A2" s="1">
+        <v>1574</v>
+      </c>
+      <c r="B2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
         <v>161</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="B3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
         <v>162</v>
       </c>
-      <c r="B3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>1574</v>
-      </c>
       <c r="B4" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>1573</v>
-      </c>
-      <c r="B5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C5" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -941,10 +875,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{209AAC4B-633B-8D4C-8F7E-1A9573C5BFCB}">
-  <dimension ref="A1:C47"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView zoomScale="127" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -954,483 +888,460 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+      <c r="B19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
+      <c r="C33" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B38" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
+      <c r="C38" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B37" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>92</v>
-      </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>92</v>
+      <c r="A39" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>92</v>
-      </c>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="3"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="3"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="3"/>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="3"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="3"/>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="3"/>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="3"/>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:B52">
-    <sortCondition ref="B1:B52"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:B49">
+    <sortCondition ref="B1:B49"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1438,89 +1349,92 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2066806-BCE0-B748-9DDB-90B46CB7534A}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView zoomScale="118" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="63.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B1" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="C1" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C2" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C3" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>84</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>85</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>91</v>
       </c>
       <c r="C5" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1531,63 +1445,56 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" t="s">
-        <v>92</v>
-      </c>
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
@@ -1625,22 +1532,10 @@
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:B21">
-    <sortCondition ref="B1:B21"/>
-    <sortCondition ref="A1:A21"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:B18">
+    <sortCondition ref="B1:B18"/>
+    <sortCondition ref="A1:A18"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>